<commit_message>
Added README and other forgotten (project) files.
</commit_message>
<xml_diff>
--- a/Gates_com_catalog_demo.xlsx
+++ b/Gates_com_catalog_demo.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,6 +1112,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>